<commit_message>
update code add new client
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest_RISE/datatest.xlsx
+++ b/src/test/resources/datatest_RISE/datatest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>EMAIL</t>
   </si>
@@ -36,39 +36,12 @@
     <t>admin@example.com</t>
   </si>
   <si>
-    <t>CUSTOMER_NAME</t>
-  </si>
-  <si>
     <t>PHONE</t>
   </si>
   <si>
     <t>WEBSITE</t>
   </si>
   <si>
-    <t>hatest</t>
-  </si>
-  <si>
-    <t>hatest@gmail.com</t>
-  </si>
-  <si>
-    <t>hatest.com.vn</t>
-  </si>
-  <si>
-    <t>0965865356</t>
-  </si>
-  <si>
-    <t>giangtest</t>
-  </si>
-  <si>
-    <t>giangtest@gmail.com</t>
-  </si>
-  <si>
-    <t>0968356987</t>
-  </si>
-  <si>
-    <t>giangtest.com</t>
-  </si>
-  <si>
     <t>user@example.com</t>
   </si>
   <si>
@@ -79,6 +52,42 @@
   </si>
   <si>
     <t>hatest2@example.com</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>COMPANY_NAME</t>
+  </si>
+  <si>
+    <t>OWNER</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>VAT</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>CLIENT GROUPS</t>
+  </si>
+  <si>
+    <t>LABELS</t>
   </si>
 </sst>
 </file>
@@ -422,14 +431,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -450,7 +459,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1253</v>
@@ -458,7 +467,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>123456</v>
@@ -466,7 +475,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>123456</v>
@@ -474,7 +483,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>123456</v>
@@ -520,67 +529,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add xpath button New contact of client
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest_RISE/datatest.xlsx
+++ b/src/test/resources/datatest_RISE/datatest.xlsx
@@ -84,10 +84,10 @@
     <t>GST</t>
   </si>
   <si>
-    <t>CLIENT GROUPS</t>
-  </si>
-  <si>
     <t>LABELS</t>
+  </si>
+  <si>
+    <t>CLIENT_GROUPS</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,10 +590,10 @@
         <v>18</v>
       </c>
       <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
         <v>19</v>
-      </c>
-      <c r="N1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>